<commit_message>
Added new tex files to output
</commit_message>
<xml_diff>
--- a/core/sample_inputs/input_financial.xlsx
+++ b/core/sample_inputs/input_financial.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Economic Assumptuions" sheetId="1" r:id="rId1"/>
-    <sheet name="Loan Disbursement Time" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Sn</t>
   </si>
@@ -87,15 +86,6 @@
   </si>
   <si>
     <t>Rate of Revenue Expenditure</t>
-  </si>
-  <si>
-    <t>Time of Loan Disbursement (in months)</t>
-  </si>
-  <si>
-    <t>Principal Loan Repayment</t>
-  </si>
-  <si>
-    <t>Disbursement at (month)</t>
   </si>
   <si>
     <t>Construction Period (months)</t>
@@ -144,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +157,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -187,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,12 +180,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD0E0E3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA2C4C9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,9 +234,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -275,17 +252,13 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -305,13 +278,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +592,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
@@ -639,7 +605,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -652,8 +618,8 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>31</v>
+      <c r="B2" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="6">
         <v>365</v>
@@ -663,7 +629,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="18"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -678,7 +644,7 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="7">
@@ -693,7 +659,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -702,7 +668,7 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
@@ -713,7 +679,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="18"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -724,7 +690,7 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
@@ -735,7 +701,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="18"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -746,8 +712,8 @@
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>36</v>
+      <c r="B10" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="6">
         <v>10</v>
@@ -757,7 +723,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="18"/>
+      <c r="B11" s="16"/>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
@@ -768,7 +734,7 @@
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="8">
@@ -779,7 +745,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="18"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -790,8 +756,8 @@
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>27</v>
+      <c r="B14" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="6">
         <v>18</v>
@@ -801,7 +767,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="18"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
@@ -812,8 +778,8 @@
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>28</v>
+      <c r="B16" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="6">
         <v>6</v>
@@ -823,7 +789,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="18"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
@@ -834,8 +800,8 @@
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>29</v>
+      <c r="B18" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="6">
         <v>3</v>
@@ -845,7 +811,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="18"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
@@ -856,8 +822,8 @@
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>32</v>
+      <c r="B20" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="C20" s="6">
         <v>20</v>
@@ -867,7 +833,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="18"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
@@ -878,7 +844,7 @@
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="7">
@@ -889,182 +855,101 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="18"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="14">
+      <c r="B24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="12">
         <v>1.88</v>
       </c>
-      <c r="D24" s="13"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="18"/>
+      <c r="B25" s="16"/>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="21">
+      <c r="B26" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="19">
         <v>0.6</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="20">
         <v>0.4</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="18"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="11"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="21">
+        <v>34</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="19">
         <v>0.15</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="18"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="21">
+        <v>36</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="19">
         <v>0.15</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-    </row>
-    <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="23">
-        <v>1000</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23">
-        <v>1</v>
-      </c>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>2</v>
-      </c>
-      <c r="B4" s="23">
-        <v>724.1</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23">
-        <v>7</v>
-      </c>
-      <c r="F4" s="23"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added report_chapter_1 and refactoring
</commit_message>
<xml_diff>
--- a/core/sample_inputs/input_financial.xlsx
+++ b/core/sample_inputs/input_financial.xlsx
@@ -140,7 +140,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +158,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -240,9 +233,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -259,12 +252,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -589,29 +580,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -624,7 +613,7 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="6">
@@ -635,7 +624,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="16"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
@@ -650,7 +639,7 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="7">
@@ -665,7 +654,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -674,7 +663,7 @@
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
@@ -685,7 +674,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
@@ -696,7 +685,7 @@
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
@@ -707,7 +696,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="16"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
@@ -718,7 +707,7 @@
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="6">
@@ -729,7 +718,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
@@ -740,7 +729,7 @@
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="6">
@@ -751,7 +740,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="16"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -762,7 +751,7 @@
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="8">
@@ -773,7 +762,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="16"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
@@ -784,7 +773,7 @@
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="6">
@@ -793,20 +782,20 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6">
@@ -815,20 +804,20 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="16"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="6">
@@ -837,20 +826,20 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="6">
@@ -859,20 +848,20 @@
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="7">
@@ -881,35 +870,31 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="16"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>1.88</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="16"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
@@ -918,63 +903,63 @@
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <v>0.6</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="18">
         <v>0.4</v>
       </c>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="16"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="17">
         <v>0.15</v>
       </c>
-      <c r="D30" s="20"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="16"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="17">
         <v>0.15</v>
       </c>
-      <c r="D32" s="20"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="5"/>
     </row>
   </sheetData>

</xml_diff>